<commit_message>
Got performer working in the ReFramework for collating consultant invoices
</commit_message>
<xml_diff>
--- a/Collate hours worked from contractors Reframework/Config/Config.xlsx
+++ b/Collate hours worked from contractors Reframework/Config/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\premal\Google Drive\QAC projects\HR automation\automation\HR-Payroll-automation\Collate hours worked from contractors Reframework\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EA655D-20AF-414F-A142-F26D18AA5E4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D6232E-9549-4B3F-B43A-1B5DDC5CC346}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -140,9 +140,6 @@
     <t>C:\\Users\\premal\\Google Drive\\QAC projects\\HR automation\\automation\\HR-Payroll-automation\\Collate hours worked from contractors Reframework\\invoices</t>
   </si>
   <si>
-    <t>C:\\Users\\premal\\Google Drive\\QAC projects\\HR automation\\automation\\HR-Payroll-automation\\Collate hours worked from contractors Reframework\\Database</t>
-  </si>
-  <si>
     <t>C:\\Users\\premal\\Google Drive\\QAC projects\\HR automation\\automation\\HR-Payroll-automation\\Collate hours worked from contractors Reframework\\Database\\International Consultants Template.xlsx</t>
   </si>
   <si>
@@ -153,6 +150,9 @@
   </si>
   <si>
     <t>Mailbox</t>
+  </si>
+  <si>
+    <t>C:\\Users\\premal\\Google Drive\\QAC projects\\HR automation\\automation\\HR-Payroll-automation\\Collate hours worked from contractors Reframework\\Database\\</t>
   </si>
 </sst>
 </file>
@@ -532,7 +532,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -593,7 +593,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>30</v>
@@ -615,7 +615,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
@@ -639,13 +639,13 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
         <v>40</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>